<commit_message>
A last migration test...
</commit_message>
<xml_diff>
--- a/MP2-Asset-tracking-EF-Ole/Docs/Seeding.xlsx
+++ b/MP2-Asset-tracking-EF-Ole/Docs/Seeding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89cb6c502d27d643/Documents/Projekt/Lexicon .NET/source/repos/MP2-Asset-tracking-EF-Ole/MP2-Asset-tracking-EF-Ole/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9C6AE38-FB31-4FAA-9EF5-CBACB6DB0A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{B9C6AE38-FB31-4FAA-9EF5-CBACB6DB0A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B48442B0-5449-4F51-A4C2-CB1BCF7CA93E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{03D50DBC-DCFF-4752-B263-0915594260E9}"/>
   </bookViews>
@@ -3944,9 +3944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDDD44A-07EF-4FD0-9E02-AA6258F8A910}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3960,7 +3958,7 @@
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="201" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="214.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4038,8 +4036,8 @@
         <v>1995, 04, 03</v>
       </c>
       <c r="L2" t="str">
-        <f>"modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="""&amp;B2&amp;""", Model="""&amp;C2&amp;""", Type="""&amp;D2&amp;""", Brand="""&amp;E2&amp;""", Id="&amp;A2&amp;", OfficeId="&amp;F2&amp;", EndOfLife=new DateTime("&amp;J2&amp;"), PurchaseDate=new DateTime("&amp;K2&amp;")});"</f>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="E7440", Type="Laptop", Brand="Dell", Id=1, OfficeId=4, EndOfLife=new DateTime(1998, 04, 03), PurchaseDate=new DateTime(1995, 04, 03)});</v>
+        <f>"modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="""&amp;B2&amp;""", Model="""&amp;C2&amp;""", Type="""&amp;D2&amp;""", Brand="""&amp;E2&amp;""", Id="&amp;A2&amp;", OfficeId="&amp;F2&amp;", EndOfLife=new DateTime("&amp;J2&amp;"), PurchaseDate=new DateTime("&amp;K2&amp;"), DollarPrice="&amp;I2&amp;"});"</f>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="E7440", Type="Laptop", Brand="Dell", Id=1, OfficeId=4, EndOfLife=new DateTime(1998, 04, 03), PurchaseDate=new DateTime(1995, 04, 03), DollarPrice=300});</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4079,8 +4077,8 @@
         <v>2019, 05, 03</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L8" si="1">"modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="""&amp;B3&amp;""", Model="""&amp;C3&amp;""", Type="""&amp;D3&amp;""", Brand="""&amp;E3&amp;""", Id="&amp;A3&amp;", OfficeId="&amp;F3&amp;", EndOfLife=new DateTime("&amp;J3&amp;"), PurchaseDate=new DateTime("&amp;K3&amp;")});"</f>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Galaxy", Model="A41", Type="Mobile", Brand="Samsung", Id=3, OfficeId=4, EndOfLife=new DateTime(2022, 05, 03), PurchaseDate=new DateTime(2019, 05, 03)});</v>
+        <f t="shared" ref="L3:L8" si="1">"modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="""&amp;B3&amp;""", Model="""&amp;C3&amp;""", Type="""&amp;D3&amp;""", Brand="""&amp;E3&amp;""", Id="&amp;A3&amp;", OfficeId="&amp;F3&amp;", EndOfLife=new DateTime("&amp;J3&amp;"), PurchaseDate=new DateTime("&amp;K3&amp;"), DollarPrice="&amp;I3&amp;"});"</f>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Galaxy", Model="A41", Type="Mobile", Brand="Samsung", Id=3, OfficeId=4, EndOfLife=new DateTime(2022, 05, 03), PurchaseDate=new DateTime(2019, 05, 03), DollarPrice=200});</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4121,7 +4119,7 @@
       </c>
       <c r="L4" t="str">
         <f t="shared" si="1"/>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Iphone", Model="13", Type="Mobile", Brand="Apple", Id=4, OfficeId=4, EndOfLife=new DateTime(2025, 09, 15), PurchaseDate=new DateTime(2022, 09, 15)});</v>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Iphone", Model="13", Type="Mobile", Brand="Apple", Id=4, OfficeId=4, EndOfLife=new DateTime(2025, 09, 15), PurchaseDate=new DateTime(2022, 09, 15), DollarPrice=600});</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4162,7 +4160,7 @@
       </c>
       <c r="L5" t="str">
         <f t="shared" si="1"/>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="iPhone", Model="14", Type="Mobile", Brand="Apple", Id=5, OfficeId=1, EndOfLife=new DateTime(2023, 03, 01), PurchaseDate=new DateTime(2023, 02, 01)});</v>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="iPhone", Model="14", Type="Mobile", Brand="Apple", Id=5, OfficeId=1, EndOfLife=new DateTime(2023, 03, 01), PurchaseDate=new DateTime(2023, 02, 01), DollarPrice=1200});</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4203,7 +4201,7 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="1"/>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="X89", Type="Laptop", Brand="IBM", Id=7, OfficeId=12, EndOfLife=new DateTime(2013, 08, 01), PurchaseDate=new DateTime(2010, 08, 01)});</v>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="X89", Type="Laptop", Brand="IBM", Id=7, OfficeId=12, EndOfLife=new DateTime(2013, 08, 01), PurchaseDate=new DateTime(2010, 08, 01), DollarPrice=800});</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4244,7 +4242,7 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="1"/>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="E7440", Type="Laptop", Brand="Dell", Id=8, OfficeId=8, EndOfLife=new DateTime(2022, 08, 01), PurchaseDate=new DateTime(2019, 08, 01)});</v>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="Latitude", Model="E7440", Type="Laptop", Brand="Dell", Id=8, OfficeId=8, EndOfLife=new DateTime(2022, 08, 01), PurchaseDate=new DateTime(2019, 08, 01), DollarPrice=200});</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4285,7 +4283,7 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="1"/>
-        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="X360", Model="i", Type="Laptop", Brand="HP", Id=9, OfficeId=2, EndOfLife=new DateTime(2022, 06, 01), PurchaseDate=new DateTime(2019, 06, 01)});</v>
+        <v>modelBuilder.Entity&lt;Asset&gt;().HasData(new Asset { Name="X360", Model="i", Type="Laptop", Brand="HP", Id=9, OfficeId=2, EndOfLife=new DateTime(2022, 06, 01), PurchaseDate=new DateTime(2019, 06, 01), DollarPrice=400});</v>
       </c>
     </row>
   </sheetData>

</xml_diff>